<commit_message>
add settings and models field
</commit_message>
<xml_diff>
--- a/uploads/ejemplo_importacion_licencias.xlsx
+++ b/uploads/ejemplo_importacion_licencias.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>4133-Período de Excedencia</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>4070-Licencia por Matrimonio</t>
+  </si>
+  <si>
+    <t>tst</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G162"/>
+  <dimension ref="A1:G163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,180 +500,180 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>2242</v>
+        <v>1111</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1">
-        <v>45216</v>
+        <v>45286</v>
       </c>
       <c r="E2" s="1">
-        <v>45305</v>
+        <v>45299</v>
       </c>
       <c r="F2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G2">
-        <v>90</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>5055</v>
+        <v>2242</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>45286</v>
+        <v>45216</v>
       </c>
       <c r="E3" s="1">
-        <v>45299</v>
+        <v>45305</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G3">
-        <v>14</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>5063</v>
+        <v>5055</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45286</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45299</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
         <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>45268</v>
-      </c>
-      <c r="E4" s="1">
-        <v>45358</v>
-      </c>
-      <c r="F4">
-        <v>24</v>
-      </c>
-      <c r="G4">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>5148</v>
+        <v>5063</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>45236</v>
+        <v>45268</v>
       </c>
       <c r="E5" s="1">
-        <v>45242</v>
+        <v>45358</v>
       </c>
       <c r="F5">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G5">
-        <v>7</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5155</v>
+        <v>5148</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>45231</v>
+        <v>45236</v>
       </c>
       <c r="E6" s="1">
-        <v>45245</v>
+        <v>45242</v>
       </c>
       <c r="F6">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>5190</v>
+        <v>5155</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
-        <v>45094</v>
+        <v>45231</v>
       </c>
       <c r="E7" s="1">
-        <v>45185</v>
+        <v>45245</v>
       </c>
       <c r="F7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>92</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>5199</v>
+        <v>5190</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>45236</v>
+        <v>45094</v>
       </c>
       <c r="E8" s="1">
-        <v>45242</v>
+        <v>45185</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G8">
-        <v>7</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>5232</v>
+        <v>5199</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="1">
-        <v>45261</v>
+        <v>45236</v>
       </c>
       <c r="E9" s="1">
-        <v>45267</v>
+        <v>45242</v>
       </c>
       <c r="F9">
         <v>7</v>
@@ -681,19 +684,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>5295</v>
+        <v>5232</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="1">
-        <v>45246</v>
+        <v>45261</v>
       </c>
       <c r="E10" s="1">
-        <v>45252</v>
+        <v>45267</v>
       </c>
       <c r="F10">
         <v>7</v>
@@ -704,25 +707,25 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>5299</v>
+        <v>5295</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="1">
-        <v>45222</v>
+        <v>45246</v>
       </c>
       <c r="E11" s="1">
-        <v>45235</v>
+        <v>45252</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G11">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -736,13 +739,13 @@
         <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>45286</v>
+        <v>45222</v>
       </c>
       <c r="E12" s="1">
-        <v>45299</v>
+        <v>45235</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G12">
         <v>14</v>
@@ -750,10 +753,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>5350</v>
+        <v>5299</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -762,33 +765,33 @@
         <v>45286</v>
       </c>
       <c r="E13" s="1">
-        <v>45292</v>
+        <v>45299</v>
       </c>
       <c r="F13">
         <v>6</v>
       </c>
       <c r="G13">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>5374</v>
+        <v>5350</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1">
-        <v>45264</v>
+        <v>45286</v>
       </c>
       <c r="E14" s="1">
-        <v>45270</v>
+        <v>45292</v>
       </c>
       <c r="F14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G14">
         <v>7</v>
@@ -796,33 +799,33 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>5392</v>
+        <v>5374</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>45229</v>
+        <v>45264</v>
       </c>
       <c r="E15" s="1">
-        <v>45242</v>
+        <v>45270</v>
       </c>
       <c r="F15">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G15">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>5412</v>
+        <v>5392</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -831,33 +834,33 @@
         <v>45229</v>
       </c>
       <c r="E16" s="1">
-        <v>45235</v>
+        <v>45242</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G16">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>5562</v>
+        <v>5412</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>45230</v>
+        <v>45229</v>
       </c>
       <c r="E17" s="1">
-        <v>45236</v>
+        <v>45235</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G17">
         <v>7</v>
@@ -865,48 +868,48 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>5563</v>
+        <v>5562</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>45015</v>
+        <v>45230</v>
       </c>
       <c r="E18" s="1">
-        <v>45194</v>
+        <v>45236</v>
       </c>
       <c r="F18">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="G18">
-        <v>180</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>5565</v>
+        <v>5563</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1">
-        <v>45251</v>
+        <v>45015</v>
       </c>
       <c r="E19" s="1">
-        <v>45257</v>
+        <v>45194</v>
       </c>
       <c r="F19">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G19">
-        <v>7</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -917,88 +920,88 @@
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D20" s="1">
-        <v>45156</v>
+        <v>45251</v>
       </c>
       <c r="E20" s="1">
-        <v>45247</v>
+        <v>45257</v>
       </c>
       <c r="F20">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G20">
-        <v>92</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>5665</v>
+        <v>5565</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>45216</v>
+        <v>45156</v>
       </c>
       <c r="E21" s="1">
-        <v>45245</v>
+        <v>45247</v>
       </c>
       <c r="F21">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G21">
-        <v>30</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>5670</v>
+        <v>5665</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1">
-        <v>45229</v>
+        <v>45216</v>
       </c>
       <c r="E22" s="1">
-        <v>45235</v>
+        <v>45245</v>
       </c>
       <c r="F22">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G22">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>5797</v>
+        <v>5670</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D23" s="1">
-        <v>45275</v>
+        <v>45229</v>
       </c>
       <c r="E23" s="1">
-        <v>45288</v>
+        <v>45235</v>
       </c>
       <c r="F23">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G23">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1009,19 +1012,19 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D24" s="1">
-        <v>45095</v>
+        <v>45275</v>
       </c>
       <c r="E24" s="1">
-        <v>45184</v>
+        <v>45288</v>
       </c>
       <c r="F24">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G24">
-        <v>90</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1035,13 +1038,13 @@
         <v>0</v>
       </c>
       <c r="D25" s="1">
-        <v>45185</v>
+        <v>45095</v>
       </c>
       <c r="E25" s="1">
-        <v>45274</v>
+        <v>45184</v>
       </c>
       <c r="F25">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="G25">
         <v>90</v>
@@ -1049,71 +1052,71 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>5850</v>
+        <v>5797</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1">
-        <v>45110</v>
+        <v>45185</v>
       </c>
       <c r="E26" s="1">
-        <v>45201</v>
+        <v>45274</v>
       </c>
       <c r="F26">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G26">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>5863</v>
+        <v>5850</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1">
-        <v>45200</v>
+        <v>45110</v>
       </c>
       <c r="E27" s="1">
-        <v>45266</v>
+        <v>45201</v>
       </c>
       <c r="F27">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G27">
-        <v>67</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>5968</v>
+        <v>5863</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1">
-        <v>45243</v>
+        <v>45200</v>
       </c>
       <c r="E28" s="1">
-        <v>45256</v>
+        <v>45266</v>
       </c>
       <c r="F28">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G28">
-        <v>14</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1124,24 +1127,43 @@
         <v>35</v>
       </c>
       <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>45243</v>
+      </c>
+      <c r="E29" s="1">
+        <v>45256</v>
+      </c>
+      <c r="F29">
+        <v>14</v>
+      </c>
+      <c r="G29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>5968</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D30" s="1">
         <v>45226</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E30" s="1">
         <v>45237</v>
       </c>
-      <c r="F29">
+      <c r="F30">
         <v>7</v>
       </c>
-      <c r="G29">
+      <c r="G30">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D31" s="1"/>
@@ -1670,6 +1692,10 @@
     <row r="162" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
+    </row>
+    <row r="163" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1">

</xml_diff>